<commit_message>
Replaced file 'DeliveryChanges.xlsx' with updated content
</commit_message>
<xml_diff>
--- a/DeliveryChanges.xlsx
+++ b/DeliveryChanges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://partnernetheb-my.sharepoint.com/personal/b578882_heb_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A322C4D-FA7C-46BB-8558-FA03C1F8E926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{895422DE-1C2B-4F8A-B6EC-2EF29478372B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{78C695A7-98F7-4B51-B9AF-BB9F9D019CA3}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{65B4762E-EB4F-440B-BDC6-30D0217F2BD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,17 +212,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,326 +549,327 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E180084-03F4-4D14-B845-067970828F39}">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC7D96F-A767-4C78-B9E1-C5F002518C31}">
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>45658</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>45658</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>45658</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>45658</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>45747</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>45747</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>206227</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>45747</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>707227705706703</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>45747</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>807227205</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>45748</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>405227404403</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>45748</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>45749</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>45750</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>45750</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>404</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>45754</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>45754</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>45754</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>227707705404</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>45755</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>205227404</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>45756</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>404205227</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>45756</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>45756</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>227705707</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>45761</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>227205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>123</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Delivery Changes via GUI
</commit_message>
<xml_diff>
--- a/DeliveryChanges.xlsx
+++ b/DeliveryChanges.xlsx
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-04-52</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -468,7 +468,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -512,7 +512,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-04-08 00:00:00</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -534,7 +534,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-04-09 00:00:00</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">

</xml_diff>